<commit_message>
updated modified files, deleted outdated list of SRA bio projects
</commit_message>
<xml_diff>
--- a/targets_SE.xlsx
+++ b/targets_SE.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7920" yWindow="1220" windowWidth="25360" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="3200" yWindow="8360" windowWidth="25600" windowHeight="16180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1439" uniqueCount="1157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1437" uniqueCount="1155">
   <si>
     <t>## 6</t>
   </si>
@@ -3481,12 +3481,6 @@
   </si>
   <si>
     <t>"# &lt;CMP&gt; CMPset1: A1-A2, A3-A4, A5-A6"</t>
-  </si>
-  <si>
-    <t>## [6]</t>
-  </si>
-  <si>
-    <t>"# &lt;CMP&gt; CMPset4:</t>
   </si>
   <si>
     <t xml:space="preserve">"# &lt;CMP&gt; CMPset3: D1-D4, D2-D5, D3-D6, D7-D10, D8-D11, D9-D12, D13-D16, D14-D17, D15-D18, D19-D22, D20-D23, D21-D24, D25-D28, D26-29, D27-D30, </t>
@@ -3985,7 +3979,7 @@
   <dimension ref="A1:F244"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4035,15 +4029,7 @@
         <v>1151</v>
       </c>
       <c r="B5" t="s">
-        <v>1156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
         <v>1154</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="7" spans="1:6">

</xml_diff>